<commit_message>
Added some exercise descriptions
</commit_message>
<xml_diff>
--- a/default_exercises.xlsx
+++ b/default_exercises.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeaumont\Documents\projects\GitHub\openWorkoutTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam-\Documents\openWorkoutTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3BC6247-0E37-41C8-8CEF-91FDCECF8E46}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF43F0FD-F34E-42AE-8022-A85989E9FC5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83C514FC-EE16-494C-95BE-F68E29AAC6C1}"/>
+    <workbookView xWindow="24330" yWindow="3345" windowWidth="28800" windowHeight="11385" xr2:uid="{83C514FC-EE16-494C-95BE-F68E29AAC6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Squat</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Begin by positioning the barbell on the floor in front of you and loading the desired amount of weight. Stand facing the barbell with your feet shoulder width apart. Grab the bar with your hands, palms facing down, by bending your knees and leaning forward from your waist. Keep your back straight during this movement, and stiffen your core as you pull ("row") the weight up to your sternum before slowly lowering it back down again. You should be in a bent-knee, forward leaning form during this entire motion, with your shoulders being brought together on your back as the weight is rowed towards you.</t>
+  </si>
+  <si>
+    <t>Begin by standing up holding a dumbell in each of your hands with your arms handing by your sides. Keep your palms facing forward during the exercise. Keep your upper arm(s) in place as you curl the dumbells up to your shoulders.</t>
+  </si>
+  <si>
+    <t>Begin by positioning the barbell on the floor in front of you and loading the desired amount of weight. Stand facing the barbell with your feet shoulder width apart, and your toes under the barbell. Keeping your feet flat, down and grab the barbell with your hands at a shoulder-width distance apart. Lift the barbell while keeping it close to your legs, with your shoulders back and your chest up. Try to prevent your back from rounding. Lift the bar to thigh level then return to the ground, in the same position it started.</t>
   </si>
 </sst>
 </file>
@@ -483,17 +489,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DB0D12-0556-43AC-AA1C-EE26BF2BA33F}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -507,7 +513,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -521,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -535,122 +541,140 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
Added some default exercises
</commit_message>
<xml_diff>
--- a/default_exercises.xlsx
+++ b/default_exercises.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam-\Documents\openWorkoutTracker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abeaumont\Documents\projects\GitHub\openWorkoutTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF43F0FD-F34E-42AE-8022-A85989E9FC5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC23223-5DC8-4C70-AC5C-2EDDA78EFE82}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24330" yWindow="3345" windowWidth="28800" windowHeight="11385" xr2:uid="{83C514FC-EE16-494C-95BE-F68E29AAC6C1}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83C514FC-EE16-494C-95BE-F68E29AAC6C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Squat</t>
   </si>
@@ -133,12 +133,15 @@
   </si>
   <si>
     <t>Begin by positioning the barbell on the floor in front of you and loading the desired amount of weight. Stand facing the barbell with your feet shoulder width apart, and your toes under the barbell. Keeping your feet flat, down and grab the barbell with your hands at a shoulder-width distance apart. Lift the barbell while keeping it close to your legs, with your shoulders back and your chest up. Try to prevent your back from rounding. Lift the bar to thigh level then return to the ground, in the same position it started.</t>
+  </si>
+  <si>
+    <t>Begin by positioning the barbell on the squat rack at a height where you can comfortably lift it on the pads of your shoulders while keeping your feet planted on the floor. Stand with your feet at shoulder width. Lift the weight off with the bar on your upper back, holding it with your hands in a position that feels easy to keep stable. Squat down by moving your hips back, trying to keep your core tense and back from rounding. You should squat until your upper leg is approximately parallel with the floor. Return to a standing position with a similar motion and repeat.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,8 +180,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{79F9EA8A-37E9-4540-9CD1-444C710223D2}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -489,17 +520,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24DB0D12-0556-43AC-AA1C-EE26BF2BA33F}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -513,7 +544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -527,7 +558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -541,7 +572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -555,17 +586,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="174.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -579,102 +610,111 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="144" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>15</v>
       </c>

</xml_diff>